<commit_message>
Update 02-06-25: Mejorado código limpieza AVP, prevalencia y proyección poblacional
</commit_message>
<xml_diff>
--- a/Bases de datos/clean/dic_arg_prev_dm.xlsx
+++ b/Bases de datos/clean/dic_arg_prev_dm.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\Desktop\Procesamiento-R\Bases de datos\clean\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{097B9686-1287-491B-8D3B-FBD186C79EA9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2BBED854-DD2E-4987-A7A7-176E7476D23C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -495,7 +495,7 @@
       <pane xSplit="1" ySplit="1" topLeftCell="B2" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="D10" sqref="D10"/>
+      <selection pane="bottomRight" activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>